<commit_message>
Added Jay and Arturo's human performance data
</commit_message>
<xml_diff>
--- a/HumanBasePerformance/Salary Predictor - Human Performance Aggregate.xlsx
+++ b/HumanBasePerformance/Salary Predictor - Human Performance Aggregate.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kershtheva/Desktop/MolecularBio-Salary-Prediction2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kershtheva/Desktop/MolecularBio-Salary-Prediction/HumanBasePerformance/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DC73C10E-5412-5C43-8844-2D329154FAE3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{477052CF-C94A-0F44-81C6-BF5D04CCF4BE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29100" yWindow="1240" windowWidth="28040" windowHeight="19180" xr2:uid="{410B02CB-55E8-A245-9F31-D183971DFD4E}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16020" xr2:uid="{410B02CB-55E8-A245-9F31-D183971DFD4E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="47">
   <si>
     <t>Job Title</t>
   </si>
@@ -515,6 +515,21 @@
   </si>
   <si>
     <t>St. Dev</t>
+  </si>
+  <si>
+    <t>Jay</t>
+  </si>
+  <si>
+    <t>Arturo</t>
+  </si>
+  <si>
+    <t>With Arturo and Jay (08/2020)</t>
+  </si>
+  <si>
+    <t>3 people (07/2020)</t>
+  </si>
+  <si>
+    <t>Average</t>
   </si>
 </sst>
 </file>
@@ -581,7 +596,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -642,6 +657,24 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -656,7 +689,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -737,6 +770,60 @@
     <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="12" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1052,10 +1139,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1233EAF-14ED-604D-8013-B502C159EA37}">
-  <dimension ref="A1:AA20"/>
+  <dimension ref="A1:AS26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R1" zoomScale="82" workbookViewId="0">
-      <selection activeCell="AG7" sqref="AG7"/>
+    <sheetView tabSelected="1" zoomScale="82" workbookViewId="0">
+      <selection activeCell="AM16" sqref="AM16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1085,9 +1172,21 @@
     <col min="25" max="25" width="14" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="10.1640625" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="14" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="14" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="14" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="14" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="16.83203125" customWidth="1"/>
+    <col min="35" max="35" width="14" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="14" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="26" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:45" ht="26" x14ac:dyDescent="0.3">
       <c r="G1" s="24" t="s">
         <v>39</v>
       </c>
@@ -1117,8 +1216,30 @@
       <c r="Y1" s="27"/>
       <c r="Z1" s="27"/>
       <c r="AA1" s="27"/>
+      <c r="AB1" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="AC1" s="28"/>
+      <c r="AD1" s="28"/>
+      <c r="AE1" s="28"/>
+      <c r="AF1" s="28"/>
+      <c r="AG1" s="28"/>
+      <c r="AH1" s="34" t="s">
+        <v>43</v>
+      </c>
+      <c r="AI1" s="34"/>
+      <c r="AJ1" s="34"/>
+      <c r="AK1" s="34"/>
+      <c r="AL1" s="34"/>
+      <c r="AM1" s="34"/>
+      <c r="AN1" s="40"/>
+      <c r="AO1" s="40"/>
+      <c r="AP1" s="40"/>
+      <c r="AQ1" s="40"/>
+      <c r="AR1" s="40"/>
+      <c r="AS1" s="40"/>
     </row>
-    <row r="2" spans="1:27" ht="26" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:45" ht="26" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
@@ -1200,8 +1321,50 @@
       <c r="AA2" s="17" t="s">
         <v>34</v>
       </c>
+      <c r="AB2" s="29" t="s">
+        <v>38</v>
+      </c>
+      <c r="AC2" s="29" t="s">
+        <v>34</v>
+      </c>
+      <c r="AD2" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="AE2" s="29" t="s">
+        <v>34</v>
+      </c>
+      <c r="AF2" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="AG2" s="29" t="s">
+        <v>34</v>
+      </c>
+      <c r="AH2" s="35" t="s">
+        <v>38</v>
+      </c>
+      <c r="AI2" s="35" t="s">
+        <v>34</v>
+      </c>
+      <c r="AJ2" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="AK2" s="35" t="s">
+        <v>34</v>
+      </c>
+      <c r="AL2" s="35" t="s">
+        <v>37</v>
+      </c>
+      <c r="AM2" s="35" t="s">
+        <v>34</v>
+      </c>
+      <c r="AN2" s="41"/>
+      <c r="AO2" s="41"/>
+      <c r="AP2" s="41"/>
+      <c r="AQ2" s="41"/>
+      <c r="AR2" s="41"/>
+      <c r="AS2" s="41"/>
     </row>
-    <row r="3" spans="1:27" s="5" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:45" s="5" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -1294,8 +1457,58 @@
         <f>1-(ABS(Z3-I3))/I3</f>
         <v>0.74257425742574257</v>
       </c>
+      <c r="AB3" s="32">
+        <v>75</v>
+      </c>
+      <c r="AC3" s="31">
+        <f>1-(ABS(AB3-G3))/G3</f>
+        <v>0.88059701492537312</v>
+      </c>
+      <c r="AD3" s="30">
+        <v>100</v>
+      </c>
+      <c r="AE3" s="31">
+        <f>1-(ABS(AD3-H3))/H3</f>
+        <v>0.7407407407407407</v>
+      </c>
+      <c r="AF3" s="30">
+        <f>(AB3+AD3)/2</f>
+        <v>87.5</v>
+      </c>
+      <c r="AG3" s="31">
+        <f>1-(ABS(AF3-I3))/I3</f>
+        <v>0.86633663366336633</v>
+      </c>
+      <c r="AH3" s="9">
+        <v>60</v>
+      </c>
+      <c r="AI3" s="36">
+        <f>1-(ABS(AH3-G3))/G3</f>
+        <v>0.89552238805970152</v>
+      </c>
+      <c r="AJ3" s="37">
+        <v>80</v>
+      </c>
+      <c r="AK3" s="36">
+        <f>1-(ABS(AJ3-H3))/H3</f>
+        <v>0.59259259259259256</v>
+      </c>
+      <c r="AL3" s="37">
+        <f>(AH3+AJ3)/2</f>
+        <v>70</v>
+      </c>
+      <c r="AM3" s="36">
+        <f>1-(ABS(AL3-I3))/I3</f>
+        <v>0.69306930693069302</v>
+      </c>
+      <c r="AN3" s="42"/>
+      <c r="AO3" s="43"/>
+      <c r="AP3" s="42"/>
+      <c r="AQ3" s="43"/>
+      <c r="AR3" s="42"/>
+      <c r="AS3" s="43"/>
     </row>
-    <row r="4" spans="1:27" s="5" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:45" s="5" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
@@ -1388,8 +1601,58 @@
         <f t="shared" ref="AA4:AA13" si="10">1-(ABS(Z4-I4))/I4</f>
         <v>0.49773755656108598</v>
       </c>
+      <c r="AB4" s="32">
+        <v>90</v>
+      </c>
+      <c r="AC4" s="31">
+        <f t="shared" ref="AC4:AC13" si="11">1-(ABS(AB4-G4))/G4</f>
+        <v>1</v>
+      </c>
+      <c r="AD4" s="30">
+        <v>120</v>
+      </c>
+      <c r="AE4" s="31">
+        <f t="shared" ref="AE4:AE13" si="12">1-(ABS(AD4-H4))/H4</f>
+        <v>0.91603053435114501</v>
+      </c>
+      <c r="AF4" s="30">
+        <f t="shared" ref="AF4:AF13" si="13">(AB4+AD4)/2</f>
+        <v>105</v>
+      </c>
+      <c r="AG4" s="31">
+        <f t="shared" ref="AG4:AG13" si="14">1-(ABS(AF4-I4))/I4</f>
+        <v>0.95022624434389136</v>
+      </c>
+      <c r="AH4" s="9">
+        <v>80</v>
+      </c>
+      <c r="AI4" s="36">
+        <f t="shared" ref="AI4:AI13" si="15">1-(ABS(AH4-G4))/G4</f>
+        <v>0.88888888888888884</v>
+      </c>
+      <c r="AJ4" s="37">
+        <v>100</v>
+      </c>
+      <c r="AK4" s="36">
+        <f t="shared" ref="AK4:AK13" si="16">1-(ABS(AJ4-H4))/H4</f>
+        <v>0.76335877862595414</v>
+      </c>
+      <c r="AL4" s="37">
+        <f t="shared" ref="AL4:AL13" si="17">(AH4+AJ4)/2</f>
+        <v>90</v>
+      </c>
+      <c r="AM4" s="36">
+        <f t="shared" ref="AM4:AM13" si="18">1-(ABS(AL4-I4))/I4</f>
+        <v>0.81447963800904977</v>
+      </c>
+      <c r="AN4" s="42"/>
+      <c r="AO4" s="43"/>
+      <c r="AP4" s="42"/>
+      <c r="AQ4" s="43"/>
+      <c r="AR4" s="42"/>
+      <c r="AS4" s="43"/>
     </row>
-    <row r="5" spans="1:27" s="5" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:45" s="5" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>11</v>
       </c>
@@ -1482,8 +1745,58 @@
         <f t="shared" si="10"/>
         <v>0.86363636363636365</v>
       </c>
+      <c r="AB5" s="33">
+        <v>100</v>
+      </c>
+      <c r="AC5" s="31">
+        <f t="shared" si="11"/>
+        <v>0.95238095238095233</v>
+      </c>
+      <c r="AD5" s="30">
+        <v>130</v>
+      </c>
+      <c r="AE5" s="31">
+        <f t="shared" si="12"/>
+        <v>0.86956521739130432</v>
+      </c>
+      <c r="AF5" s="30">
+        <f t="shared" si="13"/>
+        <v>115</v>
+      </c>
+      <c r="AG5" s="31">
+        <f t="shared" si="14"/>
+        <v>0.95454545454545459</v>
+      </c>
+      <c r="AH5" s="38">
+        <v>60</v>
+      </c>
+      <c r="AI5" s="36">
+        <f t="shared" si="15"/>
+        <v>0.5714285714285714</v>
+      </c>
+      <c r="AJ5" s="37">
+        <v>80</v>
+      </c>
+      <c r="AK5" s="36">
+        <f t="shared" si="16"/>
+        <v>0.69565217391304346</v>
+      </c>
+      <c r="AL5" s="37">
+        <f t="shared" si="17"/>
+        <v>70</v>
+      </c>
+      <c r="AM5" s="36">
+        <f t="shared" si="18"/>
+        <v>0.63636363636363635</v>
+      </c>
+      <c r="AN5" s="42"/>
+      <c r="AO5" s="43"/>
+      <c r="AP5" s="42"/>
+      <c r="AQ5" s="43"/>
+      <c r="AR5" s="42"/>
+      <c r="AS5" s="43"/>
     </row>
-    <row r="6" spans="1:27" s="5" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:45" s="5" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>13</v>
       </c>
@@ -1576,8 +1889,58 @@
         <f t="shared" si="10"/>
         <v>0.76642335766423364</v>
       </c>
+      <c r="AB6" s="32">
+        <v>140</v>
+      </c>
+      <c r="AC6" s="31">
+        <f t="shared" si="11"/>
+        <v>0.90625</v>
+      </c>
+      <c r="AD6" s="30">
+        <v>160</v>
+      </c>
+      <c r="AE6" s="31">
+        <f t="shared" si="12"/>
+        <v>0.90410958904109595</v>
+      </c>
+      <c r="AF6" s="30">
+        <f t="shared" si="13"/>
+        <v>150</v>
+      </c>
+      <c r="AG6" s="31">
+        <f t="shared" si="14"/>
+        <v>0.9051094890510949</v>
+      </c>
+      <c r="AH6" s="9">
+        <v>110</v>
+      </c>
+      <c r="AI6" s="36">
+        <f t="shared" si="15"/>
+        <v>0.859375</v>
+      </c>
+      <c r="AJ6" s="37">
+        <v>150</v>
+      </c>
+      <c r="AK6" s="36">
+        <f t="shared" si="16"/>
+        <v>0.9726027397260274</v>
+      </c>
+      <c r="AL6" s="37">
+        <f t="shared" si="17"/>
+        <v>130</v>
+      </c>
+      <c r="AM6" s="36">
+        <f t="shared" si="18"/>
+        <v>0.94890510948905105</v>
+      </c>
+      <c r="AN6" s="42"/>
+      <c r="AO6" s="43"/>
+      <c r="AP6" s="42"/>
+      <c r="AQ6" s="43"/>
+      <c r="AR6" s="42"/>
+      <c r="AS6" s="43"/>
     </row>
-    <row r="7" spans="1:27" s="5" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:45" s="5" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>16</v>
       </c>
@@ -1670,8 +2033,58 @@
         <f t="shared" si="10"/>
         <v>0.62903225806451613</v>
       </c>
+      <c r="AB7" s="32">
+        <v>150</v>
+      </c>
+      <c r="AC7" s="31">
+        <f t="shared" si="11"/>
+        <v>-1.4090909090909092</v>
+      </c>
+      <c r="AD7" s="30">
+        <v>180</v>
+      </c>
+      <c r="AE7" s="31">
+        <f t="shared" si="12"/>
+        <v>-0.25</v>
+      </c>
+      <c r="AF7" s="30">
+        <f t="shared" si="13"/>
+        <v>165</v>
+      </c>
+      <c r="AG7" s="31">
+        <f t="shared" si="14"/>
+        <v>-0.66129032258064524</v>
+      </c>
+      <c r="AH7" s="9">
+        <v>80</v>
+      </c>
+      <c r="AI7" s="36">
+        <f t="shared" si="15"/>
+        <v>0.18181818181818177</v>
+      </c>
+      <c r="AJ7" s="37">
+        <v>110</v>
+      </c>
+      <c r="AK7" s="36">
+        <f t="shared" si="16"/>
+        <v>0.625</v>
+      </c>
+      <c r="AL7" s="37">
+        <f t="shared" si="17"/>
+        <v>95</v>
+      </c>
+      <c r="AM7" s="36">
+        <f t="shared" si="18"/>
+        <v>0.467741935483871</v>
+      </c>
+      <c r="AN7" s="42"/>
+      <c r="AO7" s="43"/>
+      <c r="AP7" s="42"/>
+      <c r="AQ7" s="43"/>
+      <c r="AR7" s="42"/>
+      <c r="AS7" s="43"/>
     </row>
-    <row r="8" spans="1:27" s="5" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:45" s="5" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>18</v>
       </c>
@@ -1764,8 +2177,58 @@
         <f t="shared" si="10"/>
         <v>0.81818181818181812</v>
       </c>
+      <c r="AB8" s="32">
+        <v>80</v>
+      </c>
+      <c r="AC8" s="31">
+        <f t="shared" si="11"/>
+        <v>-5.1282051282051322E-2</v>
+      </c>
+      <c r="AD8" s="30">
+        <v>100</v>
+      </c>
+      <c r="AE8" s="31">
+        <f t="shared" si="12"/>
+        <v>0.59154929577464788</v>
+      </c>
+      <c r="AF8" s="30">
+        <f t="shared" si="13"/>
+        <v>90</v>
+      </c>
+      <c r="AG8" s="31">
+        <f t="shared" si="14"/>
+        <v>0.36363636363636365</v>
+      </c>
+      <c r="AH8" s="9">
+        <v>40</v>
+      </c>
+      <c r="AI8" s="36">
+        <f t="shared" si="15"/>
+        <v>0.97435897435897434</v>
+      </c>
+      <c r="AJ8" s="37">
+        <v>50</v>
+      </c>
+      <c r="AK8" s="36">
+        <f t="shared" si="16"/>
+        <v>0.70422535211267601</v>
+      </c>
+      <c r="AL8" s="37">
+        <f t="shared" si="17"/>
+        <v>45</v>
+      </c>
+      <c r="AM8" s="36">
+        <f t="shared" si="18"/>
+        <v>0.81818181818181812</v>
+      </c>
+      <c r="AN8" s="42"/>
+      <c r="AO8" s="43"/>
+      <c r="AP8" s="42"/>
+      <c r="AQ8" s="43"/>
+      <c r="AR8" s="42"/>
+      <c r="AS8" s="43"/>
     </row>
-    <row r="9" spans="1:27" s="5" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:45" s="5" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>20</v>
       </c>
@@ -1858,8 +2321,58 @@
         <f t="shared" si="10"/>
         <v>0.69565217391304346</v>
       </c>
+      <c r="AB9" s="32">
+        <v>45</v>
+      </c>
+      <c r="AC9" s="31">
+        <f t="shared" si="11"/>
+        <v>0.19999999999999996</v>
+      </c>
+      <c r="AD9" s="30">
+        <v>75</v>
+      </c>
+      <c r="AE9" s="31">
+        <f t="shared" si="12"/>
+        <v>0.29545454545454541</v>
+      </c>
+      <c r="AF9" s="30">
+        <f t="shared" si="13"/>
+        <v>60</v>
+      </c>
+      <c r="AG9" s="31">
+        <f t="shared" si="14"/>
+        <v>0.26086956521739135</v>
+      </c>
+      <c r="AH9" s="9">
+        <v>50</v>
+      </c>
+      <c r="AI9" s="36">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AJ9" s="37">
+        <v>70</v>
+      </c>
+      <c r="AK9" s="36">
+        <f t="shared" si="16"/>
+        <v>0.40909090909090906</v>
+      </c>
+      <c r="AL9" s="37">
+        <f t="shared" si="17"/>
+        <v>60</v>
+      </c>
+      <c r="AM9" s="36">
+        <f t="shared" si="18"/>
+        <v>0.26086956521739135</v>
+      </c>
+      <c r="AN9" s="42"/>
+      <c r="AO9" s="43"/>
+      <c r="AP9" s="42"/>
+      <c r="AQ9" s="43"/>
+      <c r="AR9" s="42"/>
+      <c r="AS9" s="43"/>
     </row>
-    <row r="10" spans="1:27" s="5" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:45" s="5" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>22</v>
       </c>
@@ -1952,8 +2465,58 @@
         <f t="shared" si="10"/>
         <v>0.96491228070175439</v>
       </c>
+      <c r="AB10" s="32">
+        <v>60</v>
+      </c>
+      <c r="AC10" s="31">
+        <f t="shared" si="11"/>
+        <v>0.33333333333333337</v>
+      </c>
+      <c r="AD10" s="30">
+        <v>90</v>
+      </c>
+      <c r="AE10" s="31">
+        <f t="shared" si="12"/>
+        <v>0.84615384615384615</v>
+      </c>
+      <c r="AF10" s="30">
+        <f t="shared" si="13"/>
+        <v>75</v>
+      </c>
+      <c r="AG10" s="31">
+        <f t="shared" si="14"/>
+        <v>0.68421052631578949</v>
+      </c>
+      <c r="AH10" s="9">
+        <v>35</v>
+      </c>
+      <c r="AI10" s="36">
+        <f t="shared" si="15"/>
+        <v>0.97222222222222221</v>
+      </c>
+      <c r="AJ10" s="37">
+        <v>45</v>
+      </c>
+      <c r="AK10" s="36">
+        <f t="shared" si="16"/>
+        <v>0.57692307692307687</v>
+      </c>
+      <c r="AL10" s="37">
+        <f t="shared" si="17"/>
+        <v>40</v>
+      </c>
+      <c r="AM10" s="36">
+        <f t="shared" si="18"/>
+        <v>0.70175438596491224</v>
+      </c>
+      <c r="AN10" s="42"/>
+      <c r="AO10" s="43"/>
+      <c r="AP10" s="42"/>
+      <c r="AQ10" s="43"/>
+      <c r="AR10" s="42"/>
+      <c r="AS10" s="43"/>
     </row>
-    <row r="11" spans="1:27" s="5" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:45" s="5" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>25</v>
       </c>
@@ -1986,7 +2549,7 @@
         <v>60</v>
       </c>
       <c r="K11" s="11">
-        <f t="shared" ref="K11:K13" si="11">1-(ABS(J11-G11))/G11</f>
+        <f t="shared" ref="K11:K13" si="19">1-(ABS(J11-G11))/G11</f>
         <v>0.82191780821917804</v>
       </c>
       <c r="L11" s="10">
@@ -2046,8 +2609,58 @@
         <f t="shared" si="10"/>
         <v>0.79754601226993871</v>
       </c>
+      <c r="AB11" s="32">
+        <v>75</v>
+      </c>
+      <c r="AC11" s="31">
+        <f t="shared" si="11"/>
+        <v>0.9726027397260274</v>
+      </c>
+      <c r="AD11" s="30">
+        <v>100</v>
+      </c>
+      <c r="AE11" s="31">
+        <f t="shared" si="12"/>
+        <v>0.88888888888888884</v>
+      </c>
+      <c r="AF11" s="30">
+        <f t="shared" si="13"/>
+        <v>87.5</v>
+      </c>
+      <c r="AG11" s="31">
+        <f t="shared" si="14"/>
+        <v>0.92638036809815949</v>
+      </c>
+      <c r="AH11" s="9">
+        <v>70</v>
+      </c>
+      <c r="AI11" s="36">
+        <f t="shared" si="15"/>
+        <v>0.95890410958904115</v>
+      </c>
+      <c r="AJ11" s="37">
+        <v>100</v>
+      </c>
+      <c r="AK11" s="36">
+        <f t="shared" si="16"/>
+        <v>0.88888888888888884</v>
+      </c>
+      <c r="AL11" s="37">
+        <f t="shared" si="17"/>
+        <v>85</v>
+      </c>
+      <c r="AM11" s="36">
+        <f t="shared" si="18"/>
+        <v>0.95705521472392641</v>
+      </c>
+      <c r="AN11" s="42"/>
+      <c r="AO11" s="43"/>
+      <c r="AP11" s="42"/>
+      <c r="AQ11" s="43"/>
+      <c r="AR11" s="42"/>
+      <c r="AS11" s="43"/>
     </row>
-    <row r="12" spans="1:27" s="5" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:45" s="5" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>27</v>
       </c>
@@ -2080,7 +2693,7 @@
         <v>80</v>
       </c>
       <c r="K12" s="11">
-        <f t="shared" si="11"/>
+        <f t="shared" si="19"/>
         <v>0.84057971014492749</v>
       </c>
       <c r="L12" s="10">
@@ -2140,8 +2753,58 @@
         <f t="shared" si="10"/>
         <v>0.39743589743589747</v>
       </c>
+      <c r="AB12" s="32">
+        <v>120</v>
+      </c>
+      <c r="AC12" s="31">
+        <f t="shared" si="11"/>
+        <v>0.26086956521739135</v>
+      </c>
+      <c r="AD12" s="30">
+        <v>150</v>
+      </c>
+      <c r="AE12" s="31">
+        <f t="shared" si="12"/>
+        <v>0.27586206896551724</v>
+      </c>
+      <c r="AF12" s="30">
+        <f t="shared" si="13"/>
+        <v>135</v>
+      </c>
+      <c r="AG12" s="31">
+        <f t="shared" si="14"/>
+        <v>0.26923076923076927</v>
+      </c>
+      <c r="AH12" s="9">
+        <v>100</v>
+      </c>
+      <c r="AI12" s="36">
+        <f t="shared" si="15"/>
+        <v>0.55072463768115942</v>
+      </c>
+      <c r="AJ12" s="37">
+        <v>120</v>
+      </c>
+      <c r="AK12" s="36">
+        <f t="shared" si="16"/>
+        <v>0.62068965517241381</v>
+      </c>
+      <c r="AL12" s="37">
+        <f t="shared" si="17"/>
+        <v>110</v>
+      </c>
+      <c r="AM12" s="36">
+        <f t="shared" si="18"/>
+        <v>0.58974358974358976</v>
+      </c>
+      <c r="AN12" s="42"/>
+      <c r="AO12" s="43"/>
+      <c r="AP12" s="42"/>
+      <c r="AQ12" s="43"/>
+      <c r="AR12" s="42"/>
+      <c r="AS12" s="43"/>
     </row>
-    <row r="13" spans="1:27" s="5" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:45" s="5" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>29</v>
       </c>
@@ -2174,7 +2837,7 @@
         <v>80</v>
       </c>
       <c r="K13" s="11">
-        <f t="shared" si="11"/>
+        <f t="shared" si="19"/>
         <v>0.88888888888888884</v>
       </c>
       <c r="L13" s="10">
@@ -2234,8 +2897,58 @@
         <f t="shared" si="10"/>
         <v>0.4831460674157303</v>
       </c>
+      <c r="AB13" s="32">
+        <v>100</v>
+      </c>
+      <c r="AC13" s="31">
+        <f t="shared" si="11"/>
+        <v>0.61111111111111116</v>
+      </c>
+      <c r="AD13" s="30">
+        <v>130</v>
+      </c>
+      <c r="AE13" s="31">
+        <f t="shared" si="12"/>
+        <v>0.77358490566037741</v>
+      </c>
+      <c r="AF13" s="30">
+        <f t="shared" si="13"/>
+        <v>115</v>
+      </c>
+      <c r="AG13" s="31">
+        <f t="shared" si="14"/>
+        <v>0.7078651685393258</v>
+      </c>
+      <c r="AH13" s="9">
+        <v>70</v>
+      </c>
+      <c r="AI13" s="36">
+        <f t="shared" si="15"/>
+        <v>0.97222222222222221</v>
+      </c>
+      <c r="AJ13" s="37">
+        <v>95</v>
+      </c>
+      <c r="AK13" s="36">
+        <f t="shared" si="16"/>
+        <v>0.89622641509433965</v>
+      </c>
+      <c r="AL13" s="37">
+        <f t="shared" si="17"/>
+        <v>82.5</v>
+      </c>
+      <c r="AM13" s="36">
+        <f t="shared" si="18"/>
+        <v>0.9269662921348315</v>
+      </c>
+      <c r="AN13" s="42"/>
+      <c r="AO13" s="43"/>
+      <c r="AP13" s="42"/>
+      <c r="AQ13" s="43"/>
+      <c r="AR13" s="42"/>
+      <c r="AS13" s="43"/>
     </row>
-    <row r="14" spans="1:27" s="5" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:45" s="5" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G14"/>
       <c r="H14"/>
       <c r="I14"/>
@@ -2286,8 +2999,44 @@
         <f>AVERAGE(AA3:AA13)</f>
         <v>0.6960252766609204</v>
       </c>
+      <c r="AB14" s="21"/>
+      <c r="AC14" s="19">
+        <f>AVERAGE(AC3:AC13)</f>
+        <v>0.42334288693829353</v>
+      </c>
+      <c r="AD14" s="20"/>
+      <c r="AE14" s="19">
+        <f>AVERAGE(AE3:AE13)</f>
+        <v>0.62290360294746427</v>
+      </c>
+      <c r="AF14" s="20"/>
+      <c r="AG14" s="19">
+        <f>AVERAGE(AG3:AG13)</f>
+        <v>0.56610184182372369</v>
+      </c>
+      <c r="AH14" s="21"/>
+      <c r="AI14" s="19">
+        <f>AVERAGE(AI3:AI13)</f>
+        <v>0.7114059269335421</v>
+      </c>
+      <c r="AJ14" s="20"/>
+      <c r="AK14" s="19">
+        <f>AVERAGE(AK3:AK13)</f>
+        <v>0.70411368928544737</v>
+      </c>
+      <c r="AL14" s="20"/>
+      <c r="AM14" s="19">
+        <f>AVERAGE(AM3:AM13)</f>
+        <v>0.7104664083857064</v>
+      </c>
+      <c r="AN14" s="42"/>
+      <c r="AO14" s="44"/>
+      <c r="AP14" s="45"/>
+      <c r="AQ14" s="44"/>
+      <c r="AR14" s="45"/>
+      <c r="AS14" s="44"/>
     </row>
-    <row r="15" spans="1:27" s="5" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:45" s="5" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G15"/>
       <c r="H15"/>
       <c r="I15"/>
@@ -2338,43 +3087,140 @@
         <f>STDEV(AA3:AA13)</f>
         <v>0.17635885972551327</v>
       </c>
+      <c r="AB15" s="21"/>
+      <c r="AC15" s="15">
+        <f>STDEV(AC3:AC13)</f>
+        <v>0.71127367475536329</v>
+      </c>
+      <c r="AD15" s="20"/>
+      <c r="AE15" s="15">
+        <f>STDEV(AE3:AE13)</f>
+        <v>0.37062460120817559</v>
+      </c>
+      <c r="AF15" s="20"/>
+      <c r="AG15" s="15">
+        <f>STDEV(AG3:AG13)</f>
+        <v>0.48950354464063595</v>
+      </c>
+      <c r="AH15" s="21"/>
+      <c r="AI15" s="15">
+        <f>STDEV(AI3:AI13)</f>
+        <v>0.34434249874115863</v>
+      </c>
+      <c r="AJ15" s="20"/>
+      <c r="AK15" s="15">
+        <f>STDEV(AK3:AK13)</f>
+        <v>0.16600859235265542</v>
+      </c>
+      <c r="AL15" s="20"/>
+      <c r="AM15" s="15">
+        <f>STDEV(AM3:AM13)</f>
+        <v>0.21643680002973245</v>
+      </c>
+      <c r="AN15" s="42"/>
+      <c r="AO15" s="43"/>
+      <c r="AP15" s="45"/>
+      <c r="AQ15" s="43"/>
+      <c r="AR15" s="45"/>
+      <c r="AS15" s="43"/>
     </row>
-    <row r="16" spans="1:27" ht="23" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:45" ht="23" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
+      <c r="I16" t="s">
+        <v>46</v>
+      </c>
+      <c r="J16" s="39">
+        <f>AVERAGE(K14:O14)</f>
+        <v>0.7161711209303151</v>
+      </c>
+      <c r="Q16" s="39">
+        <f>AVERAGE(R14:V14)</f>
+        <v>0.72525677217786289</v>
+      </c>
+      <c r="W16" s="39">
+        <f>AVERAGE(X14:AB14)</f>
+        <v>0.71169879635051003</v>
+      </c>
+      <c r="AC16" s="39">
+        <f>AVERAGE(AD14:AH14)</f>
+        <v>0.59450272238559398</v>
+      </c>
+      <c r="AI16" s="39">
+        <f>AVERAGE(AJ14:AN14)</f>
+        <v>0.70729004883557689</v>
+      </c>
+      <c r="AN16" s="46"/>
+      <c r="AO16" s="47"/>
+      <c r="AP16" s="46"/>
+      <c r="AQ16" s="46"/>
+      <c r="AR16" s="46"/>
+      <c r="AS16" s="46"/>
     </row>
-    <row r="18" spans="10:11" x14ac:dyDescent="0.2">
-      <c r="J18" s="22" t="s">
+    <row r="23" spans="10:14" x14ac:dyDescent="0.2">
+      <c r="J23" t="s">
+        <v>45</v>
+      </c>
+      <c r="M23" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="24" spans="10:14" x14ac:dyDescent="0.2">
+      <c r="J24" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="K18" s="23">
+      <c r="K24" s="23">
         <f>AVERAGE(K14,Q14,W14)</f>
         <v>0.64288746850299161</v>
       </c>
+      <c r="M24" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="N24" s="23">
+        <f>AVERAGE(K14,Q14,W14,AC14,AI14)</f>
+        <v>0.6126822438761621</v>
+      </c>
     </row>
-    <row r="19" spans="10:11" x14ac:dyDescent="0.2">
-      <c r="J19" s="22" t="s">
+    <row r="25" spans="10:14" x14ac:dyDescent="0.2">
+      <c r="J25" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="K19" s="23">
+      <c r="K25" s="23">
         <f>AVERAGE(M14,S14,Y14)</f>
         <v>0.73643319140626806</v>
       </c>
+      <c r="M25" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="N25" s="23">
+        <f>AVERAGE(M14,S14,Y14,AE14,AK14)</f>
+        <v>0.70726337329034317</v>
+      </c>
     </row>
-    <row r="20" spans="10:11" x14ac:dyDescent="0.2">
-      <c r="J20" s="22" t="s">
+    <row r="26" spans="10:14" x14ac:dyDescent="0.2">
+      <c r="J26" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="K20" s="23">
+      <c r="K26" s="23">
         <f>AVERAGE(O14,U14,AA14)</f>
         <v>0.71471598450928309</v>
       </c>
+      <c r="M26" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="N26" s="23">
+        <f>AVERAGE(O14,U14,AA14,AG14,AM14)</f>
+        <v>0.68414324074745592</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="7">
+    <mergeCell ref="AH1:AM1"/>
+    <mergeCell ref="AN1:AS1"/>
     <mergeCell ref="G1:I1"/>
     <mergeCell ref="J1:O1"/>
     <mergeCell ref="P1:U1"/>
     <mergeCell ref="V1:AA1"/>
+    <mergeCell ref="AB1:AG1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>